<commit_message>
added NEArctic cod and GeorgesBank cod
</commit_message>
<xml_diff>
--- a/selectivity/data/GOM_GBK_data.xlsx
+++ b/selectivity/data/GOM_GBK_data.xlsx
@@ -1,31 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jacob\github_projets\MGWG\selectivity\US_cod\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jacob\github_projets\MGWG\selectivity\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BC5EFFB-A043-49A0-976E-04D9AF99152D}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28740" windowHeight="11550" xr2:uid="{26C94129-B488-480B-9518-F9AE930F9BF1}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28740" windowHeight="11550" activeTab="1" xr2:uid="{26C94129-B488-480B-9518-F9AE930F9BF1}"/>
   </bookViews>
   <sheets>
     <sheet name="GOMCod" sheetId="1" r:id="rId1"/>
     <sheet name="GBKCod" sheetId="5" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="40">
   <si>
     <t>Mean</t>
   </si>
@@ -94,6 +100,60 @@
   <si>
     <t xml:space="preserve">Table B23b. ASAP BASE model results for stock numbers (000s) and fishing mortality (F,unweighted,  average ages 5+) at age, 1978-2011. </t>
   </si>
+  <si>
+    <t>wcatch</t>
+  </si>
+  <si>
+    <t>fatage</t>
+  </si>
+  <si>
+    <t>natage</t>
+  </si>
+  <si>
+    <t>wmature</t>
+  </si>
+  <si>
+    <t>weights-at-age</t>
+  </si>
+  <si>
+    <t>(kg)</t>
+  </si>
+  <si>
+    <t>of</t>
+  </si>
+  <si>
+    <t>the</t>
+  </si>
+  <si>
+    <t>total</t>
+  </si>
+  <si>
+    <t>catch</t>
+  </si>
+  <si>
+    <t>January</t>
+  </si>
+  <si>
+    <t>1/spawning</t>
+  </si>
+  <si>
+    <t>stock</t>
+  </si>
+  <si>
+    <t>fishing</t>
+  </si>
+  <si>
+    <t>mortality-at-age</t>
+  </si>
+  <si>
+    <t>numbers-at-age</t>
+  </si>
+  <si>
+    <t xml:space="preserve">of Atlantic cod from the Georges Bank and South stock (NAFO Division 5Z and Subarea 6), 1978-2011. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Table B12 -  Catch mean weight (kg)  at age, </t>
+  </si>
 </sst>
 </file>
 
@@ -133,7 +193,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -146,6 +206,9 @@
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -460,15 +523,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E58F0017-9749-4AB2-8BA8-2C9FE2A63A1E}">
-  <dimension ref="A1:N132"/>
+  <dimension ref="A1:S132"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A70" sqref="A70"/>
+    <sheetView topLeftCell="A91" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="O96" sqref="O96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:19">
       <c r="B1">
         <v>0</v>
       </c>
@@ -500,19 +563,43 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:19">
       <c r="A2" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="1"/>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:19">
       <c r="A3" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="1"/>
-    </row>
-    <row r="4" spans="1:14">
+      <c r="L3" t="s">
+        <v>22</v>
+      </c>
+      <c r="M3" t="s">
+        <v>0</v>
+      </c>
+      <c r="N3" t="s">
+        <v>26</v>
+      </c>
+      <c r="O3" t="s">
+        <v>27</v>
+      </c>
+      <c r="P3" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>29</v>
+      </c>
+      <c r="R3" t="s">
+        <v>30</v>
+      </c>
+      <c r="S3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19">
       <c r="A4">
         <v>1982</v>
       </c>
@@ -546,8 +633,26 @@
       <c r="K4">
         <v>15.664</v>
       </c>
-    </row>
-    <row r="5" spans="1:14">
+      <c r="L4" t="s">
+        <v>25</v>
+      </c>
+      <c r="M4" t="s">
+        <v>0</v>
+      </c>
+      <c r="N4" t="s">
+        <v>32</v>
+      </c>
+      <c r="O4" t="s">
+        <v>33</v>
+      </c>
+      <c r="P4" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19">
       <c r="A5">
         <v>1983</v>
       </c>
@@ -581,8 +686,17 @@
       <c r="K5">
         <v>13.324999999999999</v>
       </c>
-    </row>
-    <row r="6" spans="1:14">
+      <c r="L5" t="s">
+        <v>23</v>
+      </c>
+      <c r="M5" t="s">
+        <v>35</v>
+      </c>
+      <c r="N5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19">
       <c r="A6">
         <v>1984</v>
       </c>
@@ -616,9 +730,20 @@
       <c r="K6">
         <v>14.827999999999999</v>
       </c>
-      <c r="N6" s="3"/>
-    </row>
-    <row r="7" spans="1:14">
+      <c r="L6" t="s">
+        <v>24</v>
+      </c>
+      <c r="M6" t="s">
+        <v>32</v>
+      </c>
+      <c r="N6">
+        <v>1</v>
+      </c>
+      <c r="O6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19">
       <c r="A7">
         <v>1985</v>
       </c>
@@ -654,7 +779,7 @@
       </c>
       <c r="N7" s="3"/>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:19">
       <c r="A8">
         <v>1986</v>
       </c>
@@ -690,7 +815,7 @@
       </c>
       <c r="N8" s="3"/>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:19">
       <c r="A9">
         <v>1987</v>
       </c>
@@ -726,7 +851,7 @@
       </c>
       <c r="N9" s="3"/>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:19">
       <c r="A10">
         <v>1988</v>
       </c>
@@ -762,7 +887,7 @@
       </c>
       <c r="N10" s="3"/>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:19">
       <c r="A11">
         <v>1989</v>
       </c>
@@ -797,7 +922,7 @@
         <v>20.913</v>
       </c>
     </row>
-    <row r="12" spans="1:14">
+    <row r="12" spans="1:19">
       <c r="A12">
         <v>1990</v>
       </c>
@@ -832,7 +957,7 @@
         <v>18.718</v>
       </c>
     </row>
-    <row r="13" spans="1:14">
+    <row r="13" spans="1:19">
       <c r="A13">
         <v>1991</v>
       </c>
@@ -867,7 +992,7 @@
         <v>14.031000000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:14">
+    <row r="14" spans="1:19">
       <c r="A14">
         <v>1992</v>
       </c>
@@ -902,7 +1027,7 @@
         <v>14.483000000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:14">
+    <row r="15" spans="1:19">
       <c r="A15">
         <v>1993</v>
       </c>
@@ -937,7 +1062,7 @@
         <v>15.701000000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:14">
+    <row r="16" spans="1:19">
       <c r="A16">
         <v>1994</v>
       </c>
@@ -1532,7 +1657,7 @@
         <v>11.612</v>
       </c>
     </row>
-    <row r="33" spans="1:11">
+    <row r="33" spans="1:12">
       <c r="A33">
         <v>2011</v>
       </c>
@@ -1567,13 +1692,13 @@
         <v>12.984</v>
       </c>
     </row>
-    <row r="34" spans="1:11">
+    <row r="34" spans="1:12">
       <c r="A34" t="s">
         <v>5</v>
       </c>
       <c r="B34" s="1"/>
     </row>
-    <row r="35" spans="1:11">
+    <row r="35" spans="1:12">
       <c r="A35">
         <v>1982</v>
       </c>
@@ -1607,8 +1732,11 @@
       <c r="K35">
         <v>15.664</v>
       </c>
-    </row>
-    <row r="36" spans="1:11">
+      <c r="L35" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12">
       <c r="A36">
         <v>1983</v>
       </c>
@@ -1643,7 +1771,7 @@
         <v>13.324999999999999</v>
       </c>
     </row>
-    <row r="37" spans="1:11">
+    <row r="37" spans="1:12">
       <c r="A37">
         <v>1984</v>
       </c>
@@ -1678,7 +1806,7 @@
         <v>14.827999999999999</v>
       </c>
     </row>
-    <row r="38" spans="1:11">
+    <row r="38" spans="1:12">
       <c r="A38">
         <v>1985</v>
       </c>
@@ -1713,7 +1841,7 @@
         <v>13.676</v>
       </c>
     </row>
-    <row r="39" spans="1:11">
+    <row r="39" spans="1:12">
       <c r="A39">
         <v>1986</v>
       </c>
@@ -1748,7 +1876,7 @@
         <v>14.646000000000001</v>
       </c>
     </row>
-    <row r="40" spans="1:11">
+    <row r="40" spans="1:12">
       <c r="A40">
         <v>1987</v>
       </c>
@@ -1783,7 +1911,7 @@
         <v>14.582000000000001</v>
       </c>
     </row>
-    <row r="41" spans="1:11">
+    <row r="41" spans="1:12">
       <c r="A41">
         <v>1988</v>
       </c>
@@ -1818,7 +1946,7 @@
         <v>12.993</v>
       </c>
     </row>
-    <row r="42" spans="1:11">
+    <row r="42" spans="1:12">
       <c r="A42">
         <v>1989</v>
       </c>
@@ -1853,7 +1981,7 @@
         <v>20.913</v>
       </c>
     </row>
-    <row r="43" spans="1:11">
+    <row r="43" spans="1:12">
       <c r="A43">
         <v>1990</v>
       </c>
@@ -1888,7 +2016,7 @@
         <v>18.718</v>
       </c>
     </row>
-    <row r="44" spans="1:11">
+    <row r="44" spans="1:12">
       <c r="A44">
         <v>1991</v>
       </c>
@@ -1923,7 +2051,7 @@
         <v>14.06</v>
       </c>
     </row>
-    <row r="45" spans="1:11">
+    <row r="45" spans="1:12">
       <c r="A45">
         <v>1992</v>
       </c>
@@ -1958,7 +2086,7 @@
         <v>14.483000000000001</v>
       </c>
     </row>
-    <row r="46" spans="1:11">
+    <row r="46" spans="1:12">
       <c r="A46">
         <v>1993</v>
       </c>
@@ -1993,7 +2121,7 @@
         <v>15.708</v>
       </c>
     </row>
-    <row r="47" spans="1:11">
+    <row r="47" spans="1:12">
       <c r="A47">
         <v>1994</v>
       </c>
@@ -2028,7 +2156,7 @@
         <v>11.846</v>
       </c>
     </row>
-    <row r="48" spans="1:11">
+    <row r="48" spans="1:12">
       <c r="A48">
         <v>1995</v>
       </c>
@@ -2623,13 +2751,13 @@
         <v>12.994999999999999</v>
       </c>
     </row>
-    <row r="65" spans="1:11">
+    <row r="65" spans="1:12">
       <c r="A65" t="s">
         <v>12</v>
       </c>
       <c r="B65" s="1"/>
     </row>
-    <row r="66" spans="1:11">
+    <row r="66" spans="1:12">
       <c r="A66" t="s">
         <v>8</v>
       </c>
@@ -2664,7 +2792,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="67" spans="1:11">
+    <row r="67" spans="1:12">
       <c r="A67" t="s">
         <v>9</v>
       </c>
@@ -2699,7 +2827,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:11">
+    <row r="68" spans="1:12">
       <c r="A68" t="s">
         <v>10</v>
       </c>
@@ -2734,7 +2862,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:11">
+    <row r="69" spans="1:12">
       <c r="A69" t="s">
         <v>11</v>
       </c>
@@ -2769,17 +2897,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:11">
+    <row r="70" spans="1:12">
       <c r="A70" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="71" spans="1:11" ht="18" customHeight="1">
-      <c r="A71" s="2" t="s">
+    <row r="71" spans="1:12" ht="18" customHeight="1">
+      <c r="A71" s="6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="72" spans="1:11">
+    <row r="72" spans="1:12">
       <c r="A72">
         <v>1982</v>
       </c>
@@ -2810,8 +2938,11 @@
       <c r="K72">
         <v>0.73</v>
       </c>
-    </row>
-    <row r="73" spans="1:11">
+      <c r="L72" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12">
       <c r="A73">
         <v>1983</v>
       </c>
@@ -2843,7 +2974,7 @@
         <v>0.87</v>
       </c>
     </row>
-    <row r="74" spans="1:11">
+    <row r="74" spans="1:12">
       <c r="A74">
         <v>1984</v>
       </c>
@@ -2875,7 +3006,7 @@
         <v>0.78</v>
       </c>
     </row>
-    <row r="75" spans="1:11">
+    <row r="75" spans="1:12">
       <c r="A75">
         <v>1985</v>
       </c>
@@ -2907,7 +3038,7 @@
         <v>0.91</v>
       </c>
     </row>
-    <row r="76" spans="1:11">
+    <row r="76" spans="1:12">
       <c r="A76">
         <v>1986</v>
       </c>
@@ -2939,7 +3070,7 @@
         <v>0.83</v>
       </c>
     </row>
-    <row r="77" spans="1:11">
+    <row r="77" spans="1:12">
       <c r="A77">
         <v>1987</v>
       </c>
@@ -2971,7 +3102,7 @@
         <v>0.82</v>
       </c>
     </row>
-    <row r="78" spans="1:11">
+    <row r="78" spans="1:12">
       <c r="A78">
         <v>1988</v>
       </c>
@@ -3003,7 +3134,7 @@
         <v>0.62</v>
       </c>
     </row>
-    <row r="79" spans="1:11">
+    <row r="79" spans="1:12">
       <c r="A79">
         <v>1989</v>
       </c>
@@ -3035,7 +3166,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="80" spans="1:11">
+    <row r="80" spans="1:12">
       <c r="A80">
         <v>1990</v>
       </c>
@@ -3579,7 +3710,7 @@
         <v>0.78</v>
       </c>
     </row>
-    <row r="97" spans="1:11">
+    <row r="97" spans="1:12">
       <c r="A97">
         <v>2007</v>
       </c>
@@ -3611,7 +3742,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="98" spans="1:11">
+    <row r="98" spans="1:12">
       <c r="A98">
         <v>2008</v>
       </c>
@@ -3643,7 +3774,7 @@
         <v>0.94</v>
       </c>
     </row>
-    <row r="99" spans="1:11">
+    <row r="99" spans="1:12">
       <c r="A99">
         <v>2009</v>
       </c>
@@ -3675,7 +3806,7 @@
         <v>0.98</v>
       </c>
     </row>
-    <row r="100" spans="1:11">
+    <row r="100" spans="1:12">
       <c r="A100">
         <v>2010</v>
       </c>
@@ -3707,7 +3838,7 @@
         <v>0.87</v>
       </c>
     </row>
-    <row r="101" spans="1:11">
+    <row r="101" spans="1:12">
       <c r="A101">
         <v>2011</v>
       </c>
@@ -3739,12 +3870,12 @@
         <v>0.86</v>
       </c>
     </row>
-    <row r="102" spans="1:11">
+    <row r="102" spans="1:12">
       <c r="A102" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="103" spans="1:11">
+    <row r="103" spans="1:12">
       <c r="A103">
         <v>1982</v>
       </c>
@@ -3775,8 +3906,11 @@
       <c r="K103">
         <v>232</v>
       </c>
-    </row>
-    <row r="104" spans="1:11">
+      <c r="L103" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="104" spans="1:12">
       <c r="A104">
         <v>1983</v>
       </c>
@@ -3808,7 +3942,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="105" spans="1:11">
+    <row r="105" spans="1:12">
       <c r="A105">
         <v>1984</v>
       </c>
@@ -3840,7 +3974,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="106" spans="1:11">
+    <row r="106" spans="1:12">
       <c r="A106">
         <v>1985</v>
       </c>
@@ -3872,7 +4006,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="107" spans="1:11">
+    <row r="107" spans="1:12">
       <c r="A107">
         <v>1986</v>
       </c>
@@ -3904,7 +4038,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="108" spans="1:11">
+    <row r="108" spans="1:12">
       <c r="A108">
         <v>1987</v>
       </c>
@@ -3936,7 +4070,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="109" spans="1:11">
+    <row r="109" spans="1:12">
       <c r="A109">
         <v>1988</v>
       </c>
@@ -3968,7 +4102,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="110" spans="1:11">
+    <row r="110" spans="1:12">
       <c r="A110">
         <v>1989</v>
       </c>
@@ -4000,7 +4134,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="111" spans="1:11">
+    <row r="111" spans="1:12">
       <c r="A111">
         <v>1990</v>
       </c>
@@ -4032,7 +4166,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="112" spans="1:11">
+    <row r="112" spans="1:12">
       <c r="A112">
         <v>1991</v>
       </c>
@@ -4712,10 +4846,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90291BA5-3093-4416-A93D-69B2DB932EC0}">
-  <dimension ref="A1:L190"/>
+  <dimension ref="A1:L226"/>
   <sheetViews>
-    <sheetView topLeftCell="A169" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+    <sheetView tabSelected="1" topLeftCell="A184" workbookViewId="0">
+      <selection activeCell="A192" sqref="A192"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -11356,6 +11490,1236 @@
         <v>38</v>
       </c>
     </row>
+    <row r="191" spans="1:11">
+      <c r="A191" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="192" spans="1:11">
+      <c r="A192" t="s">
+        <v>38</v>
+      </c>
+      <c r="B192">
+        <v>1</v>
+      </c>
+      <c r="C192">
+        <v>2</v>
+      </c>
+      <c r="D192">
+        <v>3</v>
+      </c>
+      <c r="E192">
+        <v>4</v>
+      </c>
+      <c r="F192">
+        <v>5</v>
+      </c>
+      <c r="G192">
+        <v>6</v>
+      </c>
+      <c r="H192">
+        <v>7</v>
+      </c>
+      <c r="I192">
+        <v>8</v>
+      </c>
+      <c r="J192">
+        <v>9</v>
+      </c>
+      <c r="K192" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="193" spans="1:11">
+      <c r="A193">
+        <v>1978</v>
+      </c>
+      <c r="B193">
+        <v>0.502</v>
+      </c>
+      <c r="C193">
+        <v>1.2090000000000001</v>
+      </c>
+      <c r="D193">
+        <v>2.3519999999999999</v>
+      </c>
+      <c r="E193">
+        <v>3.3370000000000002</v>
+      </c>
+      <c r="F193">
+        <v>3.895</v>
+      </c>
+      <c r="G193">
+        <v>6.2649999999999997</v>
+      </c>
+      <c r="H193">
+        <v>6.7060000000000004</v>
+      </c>
+      <c r="I193">
+        <v>8.4939999999999998</v>
+      </c>
+      <c r="J193">
+        <v>9.673</v>
+      </c>
+      <c r="K193">
+        <v>14.074</v>
+      </c>
+    </row>
+    <row r="194" spans="1:11">
+      <c r="A194">
+        <v>1979</v>
+      </c>
+      <c r="B194">
+        <v>0.59199999999999997</v>
+      </c>
+      <c r="C194">
+        <v>1.365</v>
+      </c>
+      <c r="D194">
+        <v>1.9319999999999999</v>
+      </c>
+      <c r="E194">
+        <v>4.1529999999999996</v>
+      </c>
+      <c r="F194">
+        <v>4.82</v>
+      </c>
+      <c r="G194">
+        <v>7.0940000000000003</v>
+      </c>
+      <c r="H194">
+        <v>9.2390000000000008</v>
+      </c>
+      <c r="I194">
+        <v>10.207000000000001</v>
+      </c>
+      <c r="J194">
+        <v>9.8610000000000007</v>
+      </c>
+      <c r="K194">
+        <v>14.006</v>
+      </c>
+    </row>
+    <row r="195" spans="1:11">
+      <c r="A195">
+        <v>1980</v>
+      </c>
+      <c r="B195">
+        <v>0.57499999999999996</v>
+      </c>
+      <c r="C195">
+        <v>1.3859999999999999</v>
+      </c>
+      <c r="D195">
+        <v>2.39</v>
+      </c>
+      <c r="E195">
+        <v>3.4860000000000002</v>
+      </c>
+      <c r="F195">
+        <v>5.5019999999999998</v>
+      </c>
+      <c r="G195">
+        <v>6.774</v>
+      </c>
+      <c r="H195">
+        <v>8.234</v>
+      </c>
+      <c r="I195">
+        <v>9.7379999999999995</v>
+      </c>
+      <c r="J195">
+        <v>9.3160000000000007</v>
+      </c>
+      <c r="K195">
+        <v>14.045</v>
+      </c>
+    </row>
+    <row r="196" spans="1:11">
+      <c r="A196">
+        <v>1981</v>
+      </c>
+      <c r="B196">
+        <v>0.60699999999999998</v>
+      </c>
+      <c r="C196">
+        <v>1.41</v>
+      </c>
+      <c r="D196">
+        <v>2.3029999999999999</v>
+      </c>
+      <c r="E196">
+        <v>3.4260000000000002</v>
+      </c>
+      <c r="F196">
+        <v>4.7770000000000001</v>
+      </c>
+      <c r="G196">
+        <v>7.0880000000000001</v>
+      </c>
+      <c r="H196">
+        <v>8.4350000000000005</v>
+      </c>
+      <c r="I196">
+        <v>9.5030000000000001</v>
+      </c>
+      <c r="J196">
+        <v>13.815</v>
+      </c>
+      <c r="K196">
+        <v>17.096</v>
+      </c>
+    </row>
+    <row r="197" spans="1:11">
+      <c r="A197">
+        <v>1982</v>
+      </c>
+      <c r="B197">
+        <v>0.64600000000000002</v>
+      </c>
+      <c r="C197">
+        <v>1.3740000000000001</v>
+      </c>
+      <c r="D197">
+        <v>2.4769999999999999</v>
+      </c>
+      <c r="E197">
+        <v>3.629</v>
+      </c>
+      <c r="F197">
+        <v>5.1509999999999998</v>
+      </c>
+      <c r="G197">
+        <v>6.6379999999999999</v>
+      </c>
+      <c r="H197">
+        <v>9.1289999999999996</v>
+      </c>
+      <c r="I197">
+        <v>9.9139999999999997</v>
+      </c>
+      <c r="J197">
+        <v>12.58</v>
+      </c>
+      <c r="K197">
+        <v>15.629</v>
+      </c>
+    </row>
+    <row r="198" spans="1:11">
+      <c r="A198">
+        <v>1983</v>
+      </c>
+      <c r="B198">
+        <v>0.67200000000000004</v>
+      </c>
+      <c r="C198">
+        <v>1.4179999999999999</v>
+      </c>
+      <c r="D198">
+        <v>2.3679999999999999</v>
+      </c>
+      <c r="E198">
+        <v>3.3250000000000002</v>
+      </c>
+      <c r="F198">
+        <v>4.7830000000000004</v>
+      </c>
+      <c r="G198">
+        <v>6.3470000000000004</v>
+      </c>
+      <c r="H198">
+        <v>8.2439999999999998</v>
+      </c>
+      <c r="I198">
+        <v>10.53</v>
+      </c>
+      <c r="J198">
+        <v>11.507</v>
+      </c>
+      <c r="K198">
+        <v>15.576000000000001</v>
+      </c>
+    </row>
+    <row r="199" spans="1:11">
+      <c r="A199">
+        <v>1984</v>
+      </c>
+      <c r="B199">
+        <v>0.65300000000000002</v>
+      </c>
+      <c r="C199">
+        <v>1.522</v>
+      </c>
+      <c r="D199">
+        <v>2.464</v>
+      </c>
+      <c r="E199">
+        <v>3.66</v>
+      </c>
+      <c r="F199">
+        <v>5.016</v>
+      </c>
+      <c r="G199">
+        <v>6.4509999999999996</v>
+      </c>
+      <c r="H199">
+        <v>8.5670000000000002</v>
+      </c>
+      <c r="I199">
+        <v>9.9789999999999992</v>
+      </c>
+      <c r="J199">
+        <v>10.974</v>
+      </c>
+      <c r="K199">
+        <v>14.052</v>
+      </c>
+    </row>
+    <row r="200" spans="1:11">
+      <c r="A200">
+        <v>1985</v>
+      </c>
+      <c r="B200">
+        <v>0.71499999999999997</v>
+      </c>
+      <c r="C200">
+        <v>1.331</v>
+      </c>
+      <c r="D200">
+        <v>2.0230000000000001</v>
+      </c>
+      <c r="E200">
+        <v>3.6970000000000001</v>
+      </c>
+      <c r="F200">
+        <v>4.8819999999999997</v>
+      </c>
+      <c r="G200">
+        <v>6.2160000000000002</v>
+      </c>
+      <c r="H200">
+        <v>8.0709999999999997</v>
+      </c>
+      <c r="I200">
+        <v>10.07</v>
+      </c>
+      <c r="J200">
+        <v>11.597</v>
+      </c>
+      <c r="K200">
+        <v>13.936</v>
+      </c>
+    </row>
+    <row r="201" spans="1:11">
+      <c r="A201">
+        <v>1986</v>
+      </c>
+      <c r="B201">
+        <v>0.70399999999999996</v>
+      </c>
+      <c r="C201">
+        <v>1.383</v>
+      </c>
+      <c r="D201">
+        <v>2.3879999999999999</v>
+      </c>
+      <c r="E201">
+        <v>3.4740000000000002</v>
+      </c>
+      <c r="F201">
+        <v>5.3630000000000004</v>
+      </c>
+      <c r="G201">
+        <v>6.9640000000000004</v>
+      </c>
+      <c r="H201">
+        <v>8.5990000000000002</v>
+      </c>
+      <c r="I201">
+        <v>9.8170000000000002</v>
+      </c>
+      <c r="J201">
+        <v>12.523999999999999</v>
+      </c>
+      <c r="K201">
+        <v>14.269</v>
+      </c>
+    </row>
+    <row r="202" spans="1:11">
+      <c r="A202">
+        <v>1987</v>
+      </c>
+      <c r="B202">
+        <v>0.66900000000000004</v>
+      </c>
+      <c r="C202">
+        <v>1.427</v>
+      </c>
+      <c r="D202">
+        <v>2.4359999999999999</v>
+      </c>
+      <c r="E202">
+        <v>4.0259999999999998</v>
+      </c>
+      <c r="F202">
+        <v>5.5830000000000002</v>
+      </c>
+      <c r="G202">
+        <v>7.5940000000000003</v>
+      </c>
+      <c r="H202">
+        <v>8.6820000000000004</v>
+      </c>
+      <c r="I202">
+        <v>9.8490000000000002</v>
+      </c>
+      <c r="J202">
+        <v>11.449</v>
+      </c>
+      <c r="K202">
+        <v>15.042</v>
+      </c>
+    </row>
+    <row r="203" spans="1:11">
+      <c r="A203">
+        <v>1988</v>
+      </c>
+      <c r="B203">
+        <v>0.55600000000000005</v>
+      </c>
+      <c r="C203">
+        <v>1.41</v>
+      </c>
+      <c r="D203">
+        <v>2.2650000000000001</v>
+      </c>
+      <c r="E203">
+        <v>3.323</v>
+      </c>
+      <c r="F203">
+        <v>5.1449999999999996</v>
+      </c>
+      <c r="G203">
+        <v>6.7080000000000002</v>
+      </c>
+      <c r="H203">
+        <v>8.6739999999999995</v>
+      </c>
+      <c r="I203">
+        <v>10.051</v>
+      </c>
+      <c r="J203">
+        <v>11.462</v>
+      </c>
+      <c r="K203">
+        <v>14.488</v>
+      </c>
+    </row>
+    <row r="204" spans="1:11">
+      <c r="A204">
+        <v>1989</v>
+      </c>
+      <c r="B204">
+        <v>0.49299999999999999</v>
+      </c>
+      <c r="C204">
+        <v>1.4690000000000001</v>
+      </c>
+      <c r="D204">
+        <v>2.1339999999999999</v>
+      </c>
+      <c r="E204">
+        <v>3.6190000000000002</v>
+      </c>
+      <c r="F204">
+        <v>5.0709999999999997</v>
+      </c>
+      <c r="G204">
+        <v>6.3879999999999999</v>
+      </c>
+      <c r="H204">
+        <v>7.6109999999999998</v>
+      </c>
+      <c r="I204">
+        <v>9.6080000000000005</v>
+      </c>
+      <c r="J204">
+        <v>10.824</v>
+      </c>
+      <c r="K204">
+        <v>13.526</v>
+      </c>
+    </row>
+    <row r="205" spans="1:11">
+      <c r="A205">
+        <v>1990</v>
+      </c>
+      <c r="B205">
+        <v>0.52700000000000002</v>
+      </c>
+      <c r="C205">
+        <v>1.502</v>
+      </c>
+      <c r="D205">
+        <v>2.3839999999999999</v>
+      </c>
+      <c r="E205">
+        <v>3.456</v>
+      </c>
+      <c r="F205">
+        <v>4.782</v>
+      </c>
+      <c r="G205">
+        <v>6.1559999999999997</v>
+      </c>
+      <c r="H205">
+        <v>8.08</v>
+      </c>
+      <c r="I205">
+        <v>10.879</v>
+      </c>
+      <c r="J205">
+        <v>11.244999999999999</v>
+      </c>
+      <c r="K205">
+        <v>13.525</v>
+      </c>
+    </row>
+    <row r="206" spans="1:11">
+      <c r="A206">
+        <v>1991</v>
+      </c>
+      <c r="B206">
+        <v>0.77300000000000002</v>
+      </c>
+      <c r="C206">
+        <v>1.488</v>
+      </c>
+      <c r="D206">
+        <v>2.452</v>
+      </c>
+      <c r="E206">
+        <v>3.4140000000000001</v>
+      </c>
+      <c r="F206">
+        <v>4.681</v>
+      </c>
+      <c r="G206">
+        <v>5.8040000000000003</v>
+      </c>
+      <c r="H206">
+        <v>7.4870000000000001</v>
+      </c>
+      <c r="I206">
+        <v>9.4860000000000007</v>
+      </c>
+      <c r="J206">
+        <v>10.242000000000001</v>
+      </c>
+      <c r="K206">
+        <v>14.429</v>
+      </c>
+    </row>
+    <row r="207" spans="1:11">
+      <c r="A207">
+        <v>1992</v>
+      </c>
+      <c r="B207">
+        <v>0.78800000000000003</v>
+      </c>
+      <c r="C207">
+        <v>1.399</v>
+      </c>
+      <c r="D207">
+        <v>2.3130000000000002</v>
+      </c>
+      <c r="E207">
+        <v>3.7530000000000001</v>
+      </c>
+      <c r="F207">
+        <v>4.4349999999999996</v>
+      </c>
+      <c r="G207">
+        <v>6.0229999999999997</v>
+      </c>
+      <c r="H207">
+        <v>7</v>
+      </c>
+      <c r="I207">
+        <v>8.8729999999999993</v>
+      </c>
+      <c r="J207">
+        <v>11.305</v>
+      </c>
+      <c r="K207">
+        <v>15.712</v>
+      </c>
+    </row>
+    <row r="208" spans="1:11">
+      <c r="A208">
+        <v>1993</v>
+      </c>
+      <c r="B208">
+        <v>0.36599999999999999</v>
+      </c>
+      <c r="C208">
+        <v>1.3380000000000001</v>
+      </c>
+      <c r="D208">
+        <v>2.1509999999999998</v>
+      </c>
+      <c r="E208">
+        <v>3.0840000000000001</v>
+      </c>
+      <c r="F208">
+        <v>4.8819999999999997</v>
+      </c>
+      <c r="G208">
+        <v>5.7569999999999997</v>
+      </c>
+      <c r="H208">
+        <v>7.1890000000000001</v>
+      </c>
+      <c r="I208">
+        <v>8.6039999999999992</v>
+      </c>
+      <c r="J208">
+        <v>10.624000000000001</v>
+      </c>
+      <c r="K208">
+        <v>14.308999999999999</v>
+      </c>
+    </row>
+    <row r="209" spans="1:11">
+      <c r="A209">
+        <v>1994</v>
+      </c>
+      <c r="B209">
+        <v>0.32300000000000001</v>
+      </c>
+      <c r="C209">
+        <v>1.21</v>
+      </c>
+      <c r="D209">
+        <v>2.073</v>
+      </c>
+      <c r="E209">
+        <v>3.4129999999999998</v>
+      </c>
+      <c r="F209">
+        <v>4.5819999999999999</v>
+      </c>
+      <c r="G209">
+        <v>6.867</v>
+      </c>
+      <c r="H209">
+        <v>6.5570000000000004</v>
+      </c>
+      <c r="I209">
+        <v>8.7200000000000006</v>
+      </c>
+      <c r="J209">
+        <v>8.8070000000000004</v>
+      </c>
+      <c r="K209">
+        <v>15.728</v>
+      </c>
+    </row>
+    <row r="210" spans="1:11">
+      <c r="A210">
+        <v>1995</v>
+      </c>
+      <c r="B210">
+        <v>0.32300000000000001</v>
+      </c>
+      <c r="C210">
+        <v>1.353</v>
+      </c>
+      <c r="D210">
+        <v>1.95</v>
+      </c>
+      <c r="E210">
+        <v>3.61</v>
+      </c>
+      <c r="F210">
+        <v>5</v>
+      </c>
+      <c r="G210">
+        <v>6.306</v>
+      </c>
+      <c r="H210">
+        <v>8.3740000000000006</v>
+      </c>
+      <c r="I210">
+        <v>11.744999999999999</v>
+      </c>
+      <c r="J210">
+        <v>11.933999999999999</v>
+      </c>
+      <c r="K210">
+        <v>18.917000000000002</v>
+      </c>
+    </row>
+    <row r="211" spans="1:11">
+      <c r="A211">
+        <v>1996</v>
+      </c>
+      <c r="B211">
+        <v>0.51400000000000001</v>
+      </c>
+      <c r="C211">
+        <v>1.379</v>
+      </c>
+      <c r="D211">
+        <v>2.323</v>
+      </c>
+      <c r="E211">
+        <v>3.145</v>
+      </c>
+      <c r="F211">
+        <v>4.8019999999999996</v>
+      </c>
+      <c r="G211">
+        <v>6.3789999999999996</v>
+      </c>
+      <c r="H211">
+        <v>7.7370000000000001</v>
+      </c>
+      <c r="I211">
+        <v>9.532</v>
+      </c>
+      <c r="J211">
+        <v>11.023999999999999</v>
+      </c>
+      <c r="K211">
+        <v>10.843999999999999</v>
+      </c>
+    </row>
+    <row r="212" spans="1:11">
+      <c r="A212">
+        <v>1997</v>
+      </c>
+      <c r="B212">
+        <v>0.45400000000000001</v>
+      </c>
+      <c r="C212">
+        <v>1.4350000000000001</v>
+      </c>
+      <c r="D212">
+        <v>2.2829999999999999</v>
+      </c>
+      <c r="E212">
+        <v>3.33</v>
+      </c>
+      <c r="F212">
+        <v>3.9169999999999998</v>
+      </c>
+      <c r="G212">
+        <v>5.5289999999999999</v>
+      </c>
+      <c r="H212">
+        <v>7.6970000000000001</v>
+      </c>
+      <c r="I212">
+        <v>7.6390000000000002</v>
+      </c>
+      <c r="J212">
+        <v>11.374000000000001</v>
+      </c>
+      <c r="K212">
+        <v>11.734</v>
+      </c>
+    </row>
+    <row r="213" spans="1:11">
+      <c r="A213">
+        <v>1998</v>
+      </c>
+      <c r="B213">
+        <v>0.55100000000000005</v>
+      </c>
+      <c r="C213">
+        <v>1.4079999999999999</v>
+      </c>
+      <c r="D213">
+        <v>2.2010000000000001</v>
+      </c>
+      <c r="E213">
+        <v>3.3490000000000002</v>
+      </c>
+      <c r="F213">
+        <v>4.43</v>
+      </c>
+      <c r="G213">
+        <v>5.4180000000000001</v>
+      </c>
+      <c r="H213">
+        <v>7.8339999999999996</v>
+      </c>
+      <c r="I213">
+        <v>7.6289999999999996</v>
+      </c>
+      <c r="J213">
+        <v>11.086</v>
+      </c>
+      <c r="K213">
+        <v>13.599</v>
+      </c>
+    </row>
+    <row r="214" spans="1:11">
+      <c r="A214">
+        <v>1999</v>
+      </c>
+      <c r="B214">
+        <v>0.45100000000000001</v>
+      </c>
+      <c r="C214">
+        <v>1.361</v>
+      </c>
+      <c r="D214">
+        <v>2.1040000000000001</v>
+      </c>
+      <c r="E214">
+        <v>3.2530000000000001</v>
+      </c>
+      <c r="F214">
+        <v>4.4359999999999999</v>
+      </c>
+      <c r="G214">
+        <v>5.774</v>
+      </c>
+      <c r="H214">
+        <v>6.6429999999999998</v>
+      </c>
+      <c r="I214">
+        <v>8.2850000000000001</v>
+      </c>
+      <c r="J214">
+        <v>10.45</v>
+      </c>
+      <c r="K214">
+        <v>13.984999999999999</v>
+      </c>
+    </row>
+    <row r="215" spans="1:11">
+      <c r="A215">
+        <v>2000</v>
+      </c>
+      <c r="B215">
+        <v>0.52100000000000002</v>
+      </c>
+      <c r="C215">
+        <v>1.55</v>
+      </c>
+      <c r="D215">
+        <v>2.3559999999999999</v>
+      </c>
+      <c r="E215">
+        <v>3.35</v>
+      </c>
+      <c r="F215">
+        <v>4.4880000000000004</v>
+      </c>
+      <c r="G215">
+        <v>5.3209999999999997</v>
+      </c>
+      <c r="H215">
+        <v>6.9530000000000003</v>
+      </c>
+      <c r="I215">
+        <v>8.0809999999999995</v>
+      </c>
+      <c r="J215">
+        <v>8.4039999999999999</v>
+      </c>
+      <c r="K215">
+        <v>13.254</v>
+      </c>
+    </row>
+    <row r="216" spans="1:11">
+      <c r="A216">
+        <v>2001</v>
+      </c>
+      <c r="B216">
+        <v>0.54700000000000004</v>
+      </c>
+      <c r="C216">
+        <v>1.391</v>
+      </c>
+      <c r="D216">
+        <v>2.1819999999999999</v>
+      </c>
+      <c r="E216">
+        <v>2.9420000000000002</v>
+      </c>
+      <c r="F216">
+        <v>4.1210000000000004</v>
+      </c>
+      <c r="G216">
+        <v>5.3920000000000003</v>
+      </c>
+      <c r="H216">
+        <v>6.1079999999999997</v>
+      </c>
+      <c r="I216">
+        <v>7.8739999999999997</v>
+      </c>
+      <c r="J216">
+        <v>9.1359999999999992</v>
+      </c>
+      <c r="K216">
+        <v>11.532</v>
+      </c>
+    </row>
+    <row r="217" spans="1:11">
+      <c r="A217">
+        <v>2002</v>
+      </c>
+      <c r="B217">
+        <v>0.46200000000000002</v>
+      </c>
+      <c r="C217">
+        <v>1.4350000000000001</v>
+      </c>
+      <c r="D217">
+        <v>2.101</v>
+      </c>
+      <c r="E217">
+        <v>2.952</v>
+      </c>
+      <c r="F217">
+        <v>3.948</v>
+      </c>
+      <c r="G217">
+        <v>5.1619999999999999</v>
+      </c>
+      <c r="H217">
+        <v>6.4950000000000001</v>
+      </c>
+      <c r="I217">
+        <v>8.0850000000000009</v>
+      </c>
+      <c r="J217">
+        <v>9.2929999999999993</v>
+      </c>
+      <c r="K217">
+        <v>11.5</v>
+      </c>
+    </row>
+    <row r="218" spans="1:11">
+      <c r="A218">
+        <v>2003</v>
+      </c>
+      <c r="B218">
+        <v>0.35599999999999998</v>
+      </c>
+      <c r="C218">
+        <v>1.605</v>
+      </c>
+      <c r="D218">
+        <v>2.246</v>
+      </c>
+      <c r="E218">
+        <v>2.8809999999999998</v>
+      </c>
+      <c r="F218">
+        <v>3.8540000000000001</v>
+      </c>
+      <c r="G218">
+        <v>4.68</v>
+      </c>
+      <c r="H218">
+        <v>5.7880000000000003</v>
+      </c>
+      <c r="I218">
+        <v>7.0069999999999997</v>
+      </c>
+      <c r="J218">
+        <v>8.3650000000000002</v>
+      </c>
+      <c r="K218">
+        <v>10.138999999999999</v>
+      </c>
+    </row>
+    <row r="219" spans="1:11">
+      <c r="A219">
+        <v>2004</v>
+      </c>
+      <c r="B219">
+        <v>0.20300000000000001</v>
+      </c>
+      <c r="C219">
+        <v>1.619</v>
+      </c>
+      <c r="D219">
+        <v>2.3969999999999998</v>
+      </c>
+      <c r="E219">
+        <v>3.1</v>
+      </c>
+      <c r="F219">
+        <v>3.851</v>
+      </c>
+      <c r="G219">
+        <v>4.7990000000000004</v>
+      </c>
+      <c r="H219">
+        <v>5.6059999999999999</v>
+      </c>
+      <c r="I219">
+        <v>7.3959999999999999</v>
+      </c>
+      <c r="J219">
+        <v>8.7850000000000001</v>
+      </c>
+      <c r="K219">
+        <v>11.292999999999999</v>
+      </c>
+    </row>
+    <row r="220" spans="1:11">
+      <c r="A220">
+        <v>2005</v>
+      </c>
+      <c r="B220">
+        <v>0.26600000000000001</v>
+      </c>
+      <c r="C220">
+        <v>0.90700000000000003</v>
+      </c>
+      <c r="D220">
+        <v>2.044</v>
+      </c>
+      <c r="E220">
+        <v>2.9470000000000001</v>
+      </c>
+      <c r="F220">
+        <v>3.9009999999999998</v>
+      </c>
+      <c r="G220">
+        <v>4.5259999999999998</v>
+      </c>
+      <c r="H220">
+        <v>5.3209999999999997</v>
+      </c>
+      <c r="I220">
+        <v>8.0440000000000005</v>
+      </c>
+      <c r="J220">
+        <v>8.7639999999999993</v>
+      </c>
+      <c r="K220">
+        <v>11.381</v>
+      </c>
+    </row>
+    <row r="221" spans="1:11">
+      <c r="A221">
+        <v>2006</v>
+      </c>
+      <c r="B221">
+        <v>0.29499999999999998</v>
+      </c>
+      <c r="C221">
+        <v>1.1279999999999999</v>
+      </c>
+      <c r="D221">
+        <v>2.1789999999999998</v>
+      </c>
+      <c r="E221">
+        <v>3.1</v>
+      </c>
+      <c r="F221">
+        <v>3.6320000000000001</v>
+      </c>
+      <c r="G221">
+        <v>4.5190000000000001</v>
+      </c>
+      <c r="H221">
+        <v>6.4340000000000002</v>
+      </c>
+      <c r="I221">
+        <v>6.3819999999999997</v>
+      </c>
+      <c r="J221">
+        <v>7.383</v>
+      </c>
+      <c r="K221">
+        <v>9.0009999999999994</v>
+      </c>
+    </row>
+    <row r="222" spans="1:11">
+      <c r="A222">
+        <v>2007</v>
+      </c>
+      <c r="B222">
+        <v>0.27600000000000002</v>
+      </c>
+      <c r="C222">
+        <v>1.524</v>
+      </c>
+      <c r="D222">
+        <v>2.1059999999999999</v>
+      </c>
+      <c r="E222">
+        <v>2.81</v>
+      </c>
+      <c r="F222">
+        <v>3.5190000000000001</v>
+      </c>
+      <c r="G222">
+        <v>4.0780000000000003</v>
+      </c>
+      <c r="H222">
+        <v>5.798</v>
+      </c>
+      <c r="I222">
+        <v>6.9459999999999997</v>
+      </c>
+      <c r="J222">
+        <v>6.8490000000000002</v>
+      </c>
+      <c r="K222">
+        <v>8.6940000000000008</v>
+      </c>
+    </row>
+    <row r="223" spans="1:11">
+      <c r="A223">
+        <v>2008</v>
+      </c>
+      <c r="B223">
+        <v>0.53700000000000003</v>
+      </c>
+      <c r="C223">
+        <v>1.68</v>
+      </c>
+      <c r="D223">
+        <v>2.351</v>
+      </c>
+      <c r="E223">
+        <v>2.831</v>
+      </c>
+      <c r="F223">
+        <v>3.6459999999999999</v>
+      </c>
+      <c r="G223">
+        <v>5.391</v>
+      </c>
+      <c r="H223">
+        <v>5.6959999999999997</v>
+      </c>
+      <c r="I223">
+        <v>8.14</v>
+      </c>
+      <c r="J223">
+        <v>8.1769999999999996</v>
+      </c>
+      <c r="K223">
+        <v>10.268000000000001</v>
+      </c>
+    </row>
+    <row r="224" spans="1:11">
+      <c r="A224">
+        <v>2009</v>
+      </c>
+      <c r="B224">
+        <v>0.53100000000000003</v>
+      </c>
+      <c r="C224">
+        <v>1.387</v>
+      </c>
+      <c r="D224">
+        <v>2.1429999999999998</v>
+      </c>
+      <c r="E224">
+        <v>3.3069999999999999</v>
+      </c>
+      <c r="F224">
+        <v>3.887</v>
+      </c>
+      <c r="G224">
+        <v>4.633</v>
+      </c>
+      <c r="H224">
+        <v>6.1150000000000002</v>
+      </c>
+      <c r="I224">
+        <v>6.6219999999999999</v>
+      </c>
+      <c r="J224">
+        <v>9.3659999999999997</v>
+      </c>
+      <c r="K224">
+        <v>11.419</v>
+      </c>
+    </row>
+    <row r="225" spans="1:11">
+      <c r="A225">
+        <v>2010</v>
+      </c>
+      <c r="B225">
+        <v>0.36499999999999999</v>
+      </c>
+      <c r="C225">
+        <v>1.214</v>
+      </c>
+      <c r="D225">
+        <v>2.2080000000000002</v>
+      </c>
+      <c r="E225">
+        <v>2.875</v>
+      </c>
+      <c r="F225">
+        <v>3.6539999999999999</v>
+      </c>
+      <c r="G225">
+        <v>3.7589999999999999</v>
+      </c>
+      <c r="H225">
+        <v>4.7690000000000001</v>
+      </c>
+      <c r="I225">
+        <v>5.8890000000000002</v>
+      </c>
+      <c r="J225">
+        <v>6.1820000000000004</v>
+      </c>
+      <c r="K225">
+        <v>12.27</v>
+      </c>
+    </row>
+    <row r="226" spans="1:11">
+      <c r="A226">
+        <v>2011</v>
+      </c>
+      <c r="B226">
+        <v>0.27300000000000002</v>
+      </c>
+      <c r="C226">
+        <v>1.2310000000000001</v>
+      </c>
+      <c r="D226">
+        <v>2.2890000000000001</v>
+      </c>
+      <c r="E226">
+        <v>2.9409999999999998</v>
+      </c>
+      <c r="F226">
+        <v>3.613</v>
+      </c>
+      <c r="G226">
+        <v>4.5510000000000002</v>
+      </c>
+      <c r="H226">
+        <v>4.7779999999999996</v>
+      </c>
+      <c r="I226">
+        <v>5.73</v>
+      </c>
+      <c r="J226">
+        <v>11.302</v>
+      </c>
+      <c r="K226">
+        <v>14.11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>